<commit_message>
Mas Cambios al excel
</commit_message>
<xml_diff>
--- a/TablaG5.xlsx
+++ b/TablaG5.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="204">
   <si>
     <t>Tipo</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Guatemala</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>Servidores</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>TGU</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -202,18 +196,12 @@
     <t>192.188.1.1</t>
   </si>
   <si>
-    <t>GT</t>
-  </si>
-  <si>
     <t>192.188.1.2</t>
   </si>
   <si>
     <t>192.188.1.3</t>
   </si>
   <si>
-    <t>MIA</t>
-  </si>
-  <si>
     <t>192.188.1.4</t>
   </si>
   <si>
@@ -250,9 +238,6 @@
     <t>192.188.1.15</t>
   </si>
   <si>
-    <t>PAM</t>
-  </si>
-  <si>
     <t>192.188.1.16</t>
   </si>
   <si>
@@ -589,70 +574,70 @@
     <t>192.160.0.0/24</t>
   </si>
   <si>
-    <t>192.169.0.0</t>
-  </si>
-  <si>
-    <t>192.169.0.1</t>
-  </si>
-  <si>
-    <t>192.169.0.126</t>
-  </si>
-  <si>
     <t>192.160.0.127</t>
   </si>
   <si>
     <t>Administracion</t>
   </si>
   <si>
-    <t>192.169.0.128</t>
-  </si>
-  <si>
-    <t>192.169.0.129</t>
-  </si>
-  <si>
-    <t>192.169.0.190</t>
-  </si>
-  <si>
-    <t>192.169.0.191</t>
-  </si>
-  <si>
-    <t>192.169.0.192</t>
-  </si>
-  <si>
-    <t>192.169.0.193</t>
-  </si>
-  <si>
-    <t>192.169.0.254</t>
-  </si>
-  <si>
-    <t>192.169.0.255</t>
-  </si>
-  <si>
-    <t>192.169.1.0</t>
-  </si>
-  <si>
-    <t>192.169.1.1</t>
-  </si>
-  <si>
-    <t>192.169.1.14</t>
-  </si>
-  <si>
-    <t>192.169.1.15</t>
-  </si>
-  <si>
-    <t>192.169.1.16</t>
-  </si>
-  <si>
-    <t>192.169.1.17</t>
-  </si>
-  <si>
-    <t>192.169.1.18</t>
-  </si>
-  <si>
-    <t>192.169.1.19</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>192.160.0.128</t>
+  </si>
+  <si>
+    <t>192.160.0.192</t>
+  </si>
+  <si>
+    <t>192.160.1.0</t>
+  </si>
+  <si>
+    <t>192.160.1.16</t>
+  </si>
+  <si>
+    <t>192.160.0.1</t>
+  </si>
+  <si>
+    <t>192.160.0.129</t>
+  </si>
+  <si>
+    <t>192.160.0.193</t>
+  </si>
+  <si>
+    <t>192.160.1.1</t>
+  </si>
+  <si>
+    <t>192.160.1.17</t>
+  </si>
+  <si>
+    <t>192.160.0.126</t>
+  </si>
+  <si>
+    <t>192.160.0.190</t>
+  </si>
+  <si>
+    <t>192.160.0.254</t>
+  </si>
+  <si>
+    <t>192.160.1.14</t>
+  </si>
+  <si>
+    <t>192.160.1.18</t>
+  </si>
+  <si>
+    <t>192.160.0.191</t>
+  </si>
+  <si>
+    <t>192.160.0.255</t>
+  </si>
+  <si>
+    <t>192.160.1.15</t>
+  </si>
+  <si>
+    <t>192.160.1.19</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -937,7 +922,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,7 +997,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1028,21 +1031,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="8" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="5" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1335,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1375,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>9</v>
@@ -1408,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>9</v>
@@ -1429,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>9</v>
@@ -1450,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>9</v>
@@ -1471,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>9</v>
@@ -1492,7 +1480,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>9</v>
@@ -1513,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>9</v>
@@ -1534,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>9</v>
@@ -1555,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>9</v>
@@ -1576,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>9</v>
@@ -1593,7 +1581,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
@@ -1605,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>9</v>
@@ -1631,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>9</v>
@@ -1657,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>9</v>
@@ -1908,7 +1896,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>14</v>
@@ -1983,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>21</v>
@@ -2004,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H30" s="5" t="s">
         <v>21</v>
@@ -2025,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>21</v>
@@ -2046,7 +2034,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>21</v>
@@ -2067,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>21</v>
@@ -2088,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>21</v>
@@ -2109,7 +2097,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>21</v>
@@ -2130,7 +2118,7 @@
         <v>1</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H36" s="5" t="s">
         <v>21</v>
@@ -2151,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>21</v>
@@ -2172,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>21</v>
@@ -2193,7 +2181,7 @@
         <v>1</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>21</v>
@@ -2214,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>21</v>
@@ -2235,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>21</v>
@@ -2256,7 +2244,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H42" s="5" t="s">
         <v>21</v>
@@ -2456,7 +2444,7 @@
         <v>15</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>14</v>
@@ -2497,7 +2485,7 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
@@ -2836,7 +2824,7 @@
         <v>15</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>14</v>
@@ -2911,10 +2899,10 @@
         <v>1</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
@@ -2932,10 +2920,10 @@
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
@@ -2953,10 +2941,10 @@
         <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
@@ -2974,10 +2962,10 @@
         <v>1</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
@@ -2995,10 +2983,10 @@
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
@@ -3016,10 +3004,10 @@
         <v>1</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
@@ -3037,10 +3025,10 @@
         <v>1</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
@@ -3058,10 +3046,10 @@
         <v>1</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
@@ -3079,10 +3067,10 @@
         <v>1</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -3100,10 +3088,10 @@
         <v>1</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
@@ -3111,7 +3099,7 @@
         <v>15</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>14</v>
@@ -3123,10 +3111,10 @@
         <v>1</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
@@ -3144,10 +3132,10 @@
         <v>1</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
@@ -3156,19 +3144,19 @@
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E85" s="2">
-        <v>1</v>
-      </c>
-      <c r="F85" s="2">
-        <v>1</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H85" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
@@ -3177,19 +3165,19 @@
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E86" s="2">
+        <v>1</v>
+      </c>
+      <c r="F86" s="2">
+        <v>1</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E86" s="2">
-        <v>1</v>
-      </c>
-      <c r="F86" s="2">
-        <v>1</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H86" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -3198,19 +3186,19 @@
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2">
+        <v>1</v>
+      </c>
+      <c r="G87" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E87" s="2">
-        <v>1</v>
-      </c>
-      <c r="F87" s="2">
-        <v>1</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H87" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -3219,19 +3207,19 @@
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E88" s="2">
+        <v>1</v>
+      </c>
+      <c r="F88" s="2">
+        <v>1</v>
+      </c>
+      <c r="G88" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E88" s="2">
-        <v>1</v>
-      </c>
-      <c r="F88" s="2">
-        <v>1</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H88" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
@@ -3240,19 +3228,19 @@
       </c>
       <c r="C89" s="2"/>
       <c r="D89" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E89" s="2">
+        <v>1</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1</v>
+      </c>
+      <c r="G89" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E89" s="2">
-        <v>1</v>
-      </c>
-      <c r="F89" s="2">
-        <v>1</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H89" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
@@ -3261,19 +3249,19 @@
       </c>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1</v>
+      </c>
+      <c r="G90" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E90" s="2">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2">
-        <v>1</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H90" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -3282,19 +3270,19 @@
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E91" s="2">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2">
+        <v>1</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E91" s="2">
-        <v>1</v>
-      </c>
-      <c r="F91" s="2">
-        <v>1</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="H91" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
@@ -3312,10 +3300,10 @@
         <v>1</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
@@ -3333,10 +3321,10 @@
         <v>1</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -3354,10 +3342,10 @@
         <v>1</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
@@ -3375,10 +3363,10 @@
         <v>1</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -3396,10 +3384,10 @@
         <v>1</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -3417,10 +3405,10 @@
         <v>1</v>
       </c>
       <c r="G97" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -3438,10 +3426,10 @@
         <v>1</v>
       </c>
       <c r="G98" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -3459,10 +3447,10 @@
         <v>1</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
@@ -3470,7 +3458,7 @@
         <v>15</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D100" s="4" t="s">
         <v>14</v>
@@ -3482,10 +3470,10 @@
         <v>1</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
@@ -3503,10 +3491,10 @@
         <v>1</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -3524,10 +3512,10 @@
         <v>1</v>
       </c>
       <c r="G102" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -3545,10 +3533,10 @@
         <v>1</v>
       </c>
       <c r="G103" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
@@ -3566,10 +3554,10 @@
         <v>1</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H104" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
@@ -3587,10 +3575,10 @@
         <v>1</v>
       </c>
       <c r="G105" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
@@ -3608,10 +3596,10 @@
         <v>2</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
@@ -3629,10 +3617,10 @@
         <v>2</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
@@ -3650,10 +3638,10 @@
         <v>2</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
@@ -3671,10 +3659,10 @@
         <v>2</v>
       </c>
       <c r="G109" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
@@ -3692,10 +3680,10 @@
         <v>1</v>
       </c>
       <c r="G110" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>27</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3709,7 +3697,7 @@
   <dimension ref="B2:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3731,27 +3719,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="26" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="27"/>
+      <c r="L2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
@@ -3766,51 +3754,51 @@
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>44</v>
-      </c>
       <c r="E3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="M3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="N3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="P3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="13" t="s">
+      <c r="R3" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="P3" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q3" s="13" t="s">
+      <c r="S3" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="T3" s="13" t="s">
         <v>3</v>
@@ -3818,19 +3806,19 @@
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>48</v>
       </c>
       <c r="E4" s="12">
         <v>24</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H4" s="12">
         <v>4</v>
@@ -3840,19 +3828,19 @@
         <v>1</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="O4" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="12">
         <v>30</v>
@@ -3875,17 +3863,17 @@
         <v>23</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" s="12">
         <v>24</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="12" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="H5" s="12">
         <v>2</v>
@@ -3895,19 +3883,19 @@
         <v>2</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P5" s="12">
         <v>30</v>
@@ -3927,20 +3915,20 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" s="12">
         <v>24</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="12" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="H6" s="12">
         <v>2</v>
@@ -3950,19 +3938,19 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N6" s="12" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P6" s="12">
         <v>30</v>
@@ -3982,20 +3970,20 @@
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="12" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E7" s="12">
         <v>24</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="12" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H7" s="12">
         <v>2</v>
@@ -4005,19 +3993,19 @@
         <v>4</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" s="12">
         <v>30</v>
@@ -4040,17 +4028,17 @@
         <v>18</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="12">
         <v>24</v>
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H8" s="12">
         <v>1</v>
@@ -4060,19 +4048,19 @@
         <v>5</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P8" s="12">
         <v>30</v>
@@ -4092,20 +4080,20 @@
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B9" s="12" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9" s="12">
         <v>24</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="12" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="H9" s="12">
         <v>1</v>
@@ -4115,19 +4103,19 @@
         <v>6</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P9" s="12">
         <v>30</v>
@@ -4147,20 +4135,20 @@
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" s="12">
         <v>24</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="12">
         <v>1</v>
@@ -4170,19 +4158,19 @@
         <v>7</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P10" s="12">
         <v>30</v>
@@ -4202,20 +4190,20 @@
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" s="12">
         <v>24</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="12">
         <v>1</v>
@@ -4225,19 +4213,19 @@
         <v>8</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P11" s="12">
         <v>30</v>
@@ -4276,10 +4264,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Y46"/>
+  <dimension ref="B2:Y53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4308,27 +4296,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="B2" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="11"/>
-      <c r="G2" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="G2" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="11"/>
-      <c r="O2" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="P2" s="26"/>
+      <c r="O2" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="P2" s="27"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
@@ -4344,30 +4332,30 @@
         <v>5</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" s="11"/>
-      <c r="G3" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="36"/>
+      <c r="G3" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
       <c r="N3" s="11"/>
-      <c r="O3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>95</v>
+      <c r="O3" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="Q3" s="11"/>
       <c r="R3" s="11"/>
@@ -4381,13 +4369,13 @@
     </row>
     <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E4" s="15">
         <v>24</v>
@@ -4397,53 +4385,53 @@
         <v>4</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J4" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K4" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N4" s="11"/>
       <c r="O4" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R4" s="13" t="s">
+      <c r="S4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V4" s="13" t="s">
+      <c r="W4" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X4" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X4" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="Y4" s="13" t="s">
         <v>3</v>
@@ -4454,10 +4442,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E5" s="15">
         <v>24</v>
@@ -4489,19 +4477,19 @@
         <v>1</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="U5" s="12">
         <v>25</v>
@@ -4521,13 +4509,13 @@
     </row>
     <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E6" s="15">
         <v>24</v>
@@ -4559,19 +4547,19 @@
         <v>2</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="T6" s="12" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="U6" s="12">
         <v>26</v>
@@ -4591,13 +4579,13 @@
     </row>
     <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E7" s="15">
         <v>24</v>
@@ -4629,19 +4617,19 @@
         <v>3</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="Q7" s="18" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="R7" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="S7" s="18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="T7" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="U7" s="18">
         <v>26</v>
@@ -4664,23 +4652,23 @@
         <v>18</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E8" s="15">
         <v>24</v>
       </c>
       <c r="F8" s="11"/>
-      <c r="G8" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="29"/>
+      <c r="G8" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
       <c r="M8" s="19">
         <f>SUM(M5:M7)</f>
         <v>151</v>
@@ -4700,13 +4688,13 @@
     </row>
     <row r="9" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E9" s="15">
         <v>24</v>
@@ -4720,89 +4708,56 @@
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
     </row>
     <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E10" s="15">
         <v>8</v>
       </c>
       <c r="F10" s="11"/>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="36"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="32"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q10" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R10" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S10" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T10" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V10" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W10" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y10" s="13" t="s">
-        <v>3</v>
-      </c>
+      <c r="O10" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
     </row>
     <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E11" s="15">
         <v>24</v>
@@ -4812,56 +4767,56 @@
         <v>4</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N11" s="11"/>
-      <c r="O11" s="12">
-        <v>1</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="R11" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="S11" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="T11" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="U11" s="12">
-        <v>26</v>
-      </c>
-      <c r="V11" s="12">
-        <v>62</v>
-      </c>
-      <c r="W11" s="12">
+      <c r="O11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="X11" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y11" s="12">
-        <v>1</v>
+      <c r="T11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U11" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W11" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y11" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:25" x14ac:dyDescent="0.25">
@@ -4894,37 +4849,37 @@
       </c>
       <c r="N12" s="11"/>
       <c r="O12" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="R12" s="12" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>135</v>
+        <v>110</v>
       </c>
       <c r="U12" s="12">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="V12" s="12">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="W12" s="12">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="X12" s="12" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
       <c r="Y12" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
@@ -4957,37 +4912,37 @@
       </c>
       <c r="N13" s="11"/>
       <c r="O13" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="U13" s="12">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="V13" s="12">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="W13" s="12">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="X13" s="12" t="s">
-        <v>141</v>
+        <v>22</v>
       </c>
       <c r="Y13" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
@@ -5003,7 +4958,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J14" s="18">
         <v>10</v>
@@ -5020,22 +4975,22 @@
       </c>
       <c r="N14" s="11"/>
       <c r="O14" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="R14" s="12" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="U14" s="12">
         <v>28</v>
@@ -5044,13 +4999,13 @@
         <v>14</v>
       </c>
       <c r="W14" s="12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="X14" s="12" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="Y14" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
@@ -5082,17 +5037,39 @@
         <v>12</v>
       </c>
       <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
+      <c r="O15" s="12">
+        <v>4</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="S15" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="U15" s="12">
+        <v>28</v>
+      </c>
+      <c r="V15" s="12">
+        <v>14</v>
+      </c>
+      <c r="W15" s="12">
+        <v>10</v>
+      </c>
+      <c r="X15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y15" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
@@ -5100,25 +5077,21 @@
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="29"/>
+      <c r="G16" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="35"/>
       <c r="M16" s="19">
         <f>SUM(M12:M15)</f>
         <v>74</v>
       </c>
       <c r="N16" s="11"/>
-      <c r="O16" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="P16" s="14" t="s">
-        <v>147</v>
-      </c>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
       <c r="Q16" s="11"/>
       <c r="R16" s="11"/>
       <c r="S16" s="11"/>
@@ -5143,39 +5116,6 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
-      <c r="O17" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P17" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q17" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R17" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S17" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U17" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W17" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X17" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y17" s="13" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="18" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
@@ -5183,49 +5123,31 @@
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="11"/>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="30"/>
-      <c r="M18" s="30"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
       <c r="N18" s="11"/>
-      <c r="O18" s="12">
-        <v>1</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="R18" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="S18" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="T18" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U18" s="12">
-        <v>27</v>
-      </c>
-      <c r="V18" s="12">
-        <v>30</v>
-      </c>
-      <c r="W18" s="12">
-        <v>23</v>
-      </c>
-      <c r="X18" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y18" s="12">
-        <v>1</v>
-      </c>
+      <c r="O18" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="11"/>
     </row>
     <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" s="11"/>
@@ -5237,56 +5159,56 @@
         <v>4</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J19" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L19" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N19" s="11"/>
-      <c r="O19" s="12">
-        <v>2</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q19" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="R19" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="S19" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="T19" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U19" s="12">
-        <v>27</v>
-      </c>
-      <c r="V19" s="12">
-        <v>30</v>
-      </c>
-      <c r="W19" s="12">
-        <v>16</v>
-      </c>
-      <c r="X19" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y19" s="12">
-        <v>2</v>
+      <c r="O19" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q19" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S19" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V19" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W19" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y19" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:25" x14ac:dyDescent="0.25">
@@ -5318,17 +5240,39 @@
         <v>23</v>
       </c>
       <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
+      <c r="O20" s="12">
+        <v>1</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="R20" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="T20" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U20" s="12">
+        <v>27</v>
+      </c>
+      <c r="V20" s="12">
+        <v>30</v>
+      </c>
+      <c r="W20" s="12">
+        <v>23</v>
+      </c>
+      <c r="X20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y20" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B21" s="11"/>
@@ -5359,21 +5303,39 @@
         <v>16</v>
       </c>
       <c r="N21" s="11"/>
-      <c r="O21" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="P21" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
+      <c r="O21" s="12">
+        <v>2</v>
+      </c>
+      <c r="P21" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q21" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="R21" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="T21" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U21" s="12">
+        <v>27</v>
+      </c>
+      <c r="V21" s="12">
+        <v>30</v>
+      </c>
+      <c r="W21" s="12">
+        <v>16</v>
+      </c>
+      <c r="X21" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y21" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B22" s="11"/>
@@ -5381,52 +5343,19 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="29"/>
+      <c r="G22" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="35"/>
       <c r="M22" s="19">
         <f>SUM(M20:M21)</f>
         <v>39</v>
       </c>
       <c r="N22" s="11"/>
-      <c r="O22" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P22" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q22" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R22" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S22" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U22" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V22" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W22" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y22" s="13" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B23" s="11"/>
@@ -5442,39 +5371,6 @@
       <c r="L23" s="11"/>
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
-      <c r="O23" s="12">
-        <v>1</v>
-      </c>
-      <c r="P23" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q23" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="R23" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="S23" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="T23" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="U23" s="12">
-        <v>25</v>
-      </c>
-      <c r="V23" s="12">
-        <v>126</v>
-      </c>
-      <c r="W23" s="12">
-        <v>69</v>
-      </c>
-      <c r="X23" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y23" s="12">
-        <v>1</v>
-      </c>
     </row>
     <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B24" s="11"/>
@@ -5482,49 +5378,31 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="G24" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
-      <c r="M24" s="31"/>
+      <c r="G24" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
       <c r="N24" s="11"/>
-      <c r="O24" s="12">
-        <v>2</v>
-      </c>
-      <c r="P24" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q24" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="R24" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="S24" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="T24" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="U24" s="12">
-        <v>26</v>
-      </c>
-      <c r="V24" s="12">
-        <v>62</v>
-      </c>
-      <c r="W24" s="12">
-        <v>48</v>
-      </c>
-      <c r="X24" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y24" s="12">
-        <v>2</v>
-      </c>
+      <c r="O24" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="P24" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="11"/>
     </row>
     <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B25" s="11"/>
@@ -5536,35 +5414,57 @@
         <v>4</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J25" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
+      <c r="O25" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q25" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V25" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W25" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X25" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y25" s="13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B26" s="11"/>
@@ -5595,21 +5495,39 @@
         <v>69</v>
       </c>
       <c r="N26" s="11"/>
-      <c r="O26" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="P26" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
+      <c r="O26" s="12">
+        <v>1</v>
+      </c>
+      <c r="P26" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q26" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="R26" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="S26" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="T26" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="U26" s="12">
+        <v>25</v>
+      </c>
+      <c r="V26" s="12">
+        <v>126</v>
+      </c>
+      <c r="W26" s="12">
+        <v>69</v>
+      </c>
+      <c r="X26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y26" s="12">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
@@ -5640,38 +5558,38 @@
         <v>48</v>
       </c>
       <c r="N27" s="11"/>
-      <c r="O27" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P27" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q27" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R27" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S27" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T27" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U27" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V27" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W27" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y27" s="13" t="s">
-        <v>3</v>
+      <c r="O27" s="12">
+        <v>2</v>
+      </c>
+      <c r="P27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q27" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="R27" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="S27" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="T27" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="U27" s="12">
+        <v>26</v>
+      </c>
+      <c r="V27" s="12">
+        <v>62</v>
+      </c>
+      <c r="W27" s="12">
+        <v>48</v>
+      </c>
+      <c r="X27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y27" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:25" x14ac:dyDescent="0.25">
@@ -5680,52 +5598,19 @@
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
-      <c r="G28" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="29"/>
+      <c r="G28" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="35"/>
       <c r="M28" s="19">
         <f>SUM(M26:M27)</f>
         <v>117</v>
       </c>
       <c r="N28" s="11"/>
-      <c r="O28" s="12">
-        <v>1</v>
-      </c>
-      <c r="P28" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q28" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="R28" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="S28" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="T28" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U28" s="12">
-        <v>27</v>
-      </c>
-      <c r="V28" s="12">
-        <v>30</v>
-      </c>
-      <c r="W28" s="12">
-        <v>23</v>
-      </c>
-      <c r="X28" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y28" s="12">
-        <v>1</v>
-      </c>
     </row>
     <row r="29" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B29" s="11"/>
@@ -5741,39 +5626,6 @@
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
-      <c r="O29" s="12">
-        <v>2</v>
-      </c>
-      <c r="P29" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q29" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="R29" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="S29" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="T29" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U29" s="12">
-        <v>27</v>
-      </c>
-      <c r="V29" s="12">
-        <v>30</v>
-      </c>
-      <c r="W29" s="12">
-        <v>16</v>
-      </c>
-      <c r="X29" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="Y29" s="12">
-        <v>2</v>
-      </c>
     </row>
     <row r="30" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B30" s="11"/>
@@ -5781,18 +5633,22 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
-      <c r="K30" s="33"/>
-      <c r="L30" s="33"/>
-      <c r="M30" s="34"/>
+      <c r="G30" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="30"/>
       <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
+      <c r="O30" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="26" t="s">
+        <v>159</v>
+      </c>
       <c r="Q30" s="11"/>
       <c r="R30" s="11"/>
       <c r="S30" s="11"/>
@@ -5813,39 +5669,57 @@
         <v>4</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J31" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N31" s="11"/>
-      <c r="O31" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="P31" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
+      <c r="O31" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P31" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q31" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T31" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V31" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W31" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X31" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y31" s="13" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>
@@ -5876,38 +5750,38 @@
         <v>23</v>
       </c>
       <c r="N32" s="11"/>
-      <c r="O32" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P32" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q32" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R32" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S32" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T32" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U32" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V32" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W32" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X32" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y32" s="13" t="s">
-        <v>3</v>
+      <c r="O32" s="12">
+        <v>1</v>
+      </c>
+      <c r="P32" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="R32" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="S32" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="T32" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U32" s="12">
+        <v>27</v>
+      </c>
+      <c r="V32" s="12">
+        <v>30</v>
+      </c>
+      <c r="W32" s="12">
+        <v>23</v>
+      </c>
+      <c r="X32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y32" s="12">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:25" x14ac:dyDescent="0.25">
@@ -5940,22 +5814,22 @@
       </c>
       <c r="N33" s="11"/>
       <c r="O33" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>116</v>
+        <v>163</v>
       </c>
       <c r="Q33" s="12" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="R33" s="12" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="S33" s="12" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="T33" s="12" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="U33" s="12">
         <v>27</v>
@@ -5964,13 +5838,13 @@
         <v>30</v>
       </c>
       <c r="W33" s="12">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="X33" s="12" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="Y33" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
@@ -5979,52 +5853,19 @@
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="29"/>
+      <c r="G34" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="35"/>
       <c r="M34" s="19">
         <f>SUM(M32:M33)</f>
         <v>39</v>
       </c>
       <c r="N34" s="11"/>
-      <c r="O34" s="12">
-        <v>2</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q34" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="R34" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="S34" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="T34" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="U34" s="12">
-        <v>27</v>
-      </c>
-      <c r="V34" s="12">
-        <v>30</v>
-      </c>
-      <c r="W34" s="12">
-        <v>16</v>
-      </c>
-      <c r="X34" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y34" s="25">
-        <v>2</v>
-      </c>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35" s="11"/>
@@ -6040,17 +5881,6 @@
       <c r="L35" s="11"/>
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-      <c r="V35" s="11"/>
-      <c r="W35" s="11"/>
-      <c r="X35" s="11"/>
-      <c r="Y35" s="11"/>
     </row>
     <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B36" s="11"/>
@@ -6058,21 +5888,21 @@
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
-      <c r="G36" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
+      <c r="G36" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
       <c r="N36" s="11"/>
-      <c r="O36" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="P36" s="14" t="s">
-        <v>181</v>
+      <c r="O36" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="P36" s="26" t="s">
+        <v>168</v>
       </c>
       <c r="Q36" s="11"/>
       <c r="R36" s="11"/>
@@ -6094,53 +5924,53 @@
         <v>4</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J37" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L37" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M37" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N37" s="11"/>
       <c r="O37" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="P37" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q37" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R37" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="Q37" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R37" s="13" t="s">
+      <c r="S37" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T37" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U37" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V37" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="S37" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T37" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U37" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V37" s="13" t="s">
+      <c r="W37" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X37" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="W37" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X37" s="13" t="s">
-        <v>56</v>
       </c>
       <c r="Y37" s="13" t="s">
         <v>3</v>
@@ -6179,28 +6009,28 @@
         <v>1</v>
       </c>
       <c r="P38" s="12" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="Q38" s="12" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="R38" s="12" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="S38" s="12" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="T38" s="12" t="s">
-        <v>185</v>
+        <v>130</v>
       </c>
       <c r="U38" s="12">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="V38" s="12">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="W38" s="12">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="X38" s="12" t="s">
         <v>8</v>
@@ -6238,17 +6068,39 @@
         <v>16</v>
       </c>
       <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="11"/>
-      <c r="S39" s="11"/>
-      <c r="T39" s="11"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="11"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="11"/>
+      <c r="O39" s="12">
+        <v>2</v>
+      </c>
+      <c r="P39" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q39" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="S39" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="T39" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="U39" s="12">
+        <v>27</v>
+      </c>
+      <c r="V39" s="12">
+        <v>30</v>
+      </c>
+      <c r="W39" s="12">
+        <v>16</v>
+      </c>
+      <c r="X39" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y39" s="25">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B40" s="11"/>
@@ -6256,25 +6108,21 @@
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
-      <c r="G40" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="29"/>
+      <c r="G40" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="34"/>
+      <c r="L40" s="35"/>
       <c r="M40" s="19">
         <f>SUM(M38:M39)</f>
         <v>39</v>
       </c>
       <c r="N40" s="11"/>
-      <c r="O40" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="P40" s="14" t="s">
-        <v>186</v>
-      </c>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
       <c r="Q40" s="11"/>
       <c r="R40" s="11"/>
       <c r="S40" s="11"/>
@@ -6299,39 +6147,6 @@
       <c r="L41" s="11"/>
       <c r="M41" s="11"/>
       <c r="N41" s="11"/>
-      <c r="O41" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="P41" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q41" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="R41" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S41" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="T41" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="U41" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="V41" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="W41" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="X41" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y41" s="13" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
@@ -6339,49 +6154,31 @@
       <c r="D42" s="11"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
-      <c r="G42" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="H42" s="31"/>
-      <c r="I42" s="31"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="31"/>
-      <c r="L42" s="31"/>
-      <c r="M42" s="31"/>
+      <c r="G42" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
       <c r="N42" s="11"/>
-      <c r="O42" s="12">
-        <v>1</v>
-      </c>
-      <c r="P42" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q42" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="R42" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="S42" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="T42" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="U42" s="12">
-        <v>25</v>
-      </c>
-      <c r="V42" s="12">
-        <v>126</v>
-      </c>
-      <c r="W42" s="12">
-        <v>69</v>
-      </c>
-      <c r="X42" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="Y42" s="12">
-        <v>1</v>
-      </c>
+      <c r="O42" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P42" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="11"/>
+      <c r="U42" s="11"/>
+      <c r="V42" s="11"/>
+      <c r="W42" s="11"/>
+      <c r="X42" s="11"/>
+      <c r="Y42" s="11"/>
     </row>
     <row r="43" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
@@ -6393,56 +6190,56 @@
         <v>4</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="I43" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J43" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K43" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M43" s="13" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="N43" s="11"/>
-      <c r="O43" s="12">
-        <v>2</v>
-      </c>
-      <c r="P43" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q43" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="R43" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="S43" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="T43" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="U43" s="12">
-        <v>26</v>
-      </c>
-      <c r="V43" s="12">
-        <v>62</v>
-      </c>
-      <c r="W43" s="12">
+      <c r="O43" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P43" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="X43" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y43" s="12">
-        <v>2</v>
+      <c r="Q43" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R43" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S43" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T43" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U43" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V43" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W43" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X43" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y43" s="13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="2:25" x14ac:dyDescent="0.25">
@@ -6475,34 +6272,34 @@
       </c>
       <c r="N44" s="11"/>
       <c r="O44" s="12">
-        <v>3</v>
-      </c>
-      <c r="P44" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q44" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="R44" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="S44" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="T44" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="U44" s="18">
-        <v>26</v>
-      </c>
-      <c r="V44" s="18">
-        <v>62</v>
-      </c>
-      <c r="W44" s="18">
-        <v>34</v>
-      </c>
-      <c r="X44" s="18" t="s">
-        <v>141</v>
+        <v>1</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q44" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="R44" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="S44" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="T44" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="U44" s="12">
+        <v>29</v>
+      </c>
+      <c r="V44" s="12">
+        <v>6</v>
+      </c>
+      <c r="W44" s="12">
+        <v>4</v>
+      </c>
+      <c r="X44" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="Y44" s="12">
         <v>1</v>
@@ -6514,52 +6311,19 @@
       <c r="D45" s="11"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
-      <c r="G45" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="29"/>
+      <c r="G45" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="35"/>
       <c r="M45" s="19">
         <f>SUM(M44:M44)</f>
         <v>4</v>
       </c>
       <c r="N45" s="11"/>
-      <c r="O45" s="12">
-        <v>4</v>
-      </c>
-      <c r="P45" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q45" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="R45" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="S45" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="T45" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="U45" s="18">
-        <v>28</v>
-      </c>
-      <c r="V45" s="18">
-        <v>14</v>
-      </c>
-      <c r="W45" s="18">
-        <v>10</v>
-      </c>
-      <c r="X45" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y45" s="12">
-        <v>2</v>
-      </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
@@ -6575,42 +6339,348 @@
       <c r="L46" s="11"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
-      <c r="O46" s="12">
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="G47" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="32"/>
+      <c r="O47" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="P47" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
+      <c r="V47" s="11"/>
+      <c r="W47" s="11"/>
+      <c r="X47" s="11"/>
+      <c r="Y47" s="11"/>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="G48" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="L48" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="M48" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="O48" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P48" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q48" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="R48" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S48" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="T48" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="U48" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="V48" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="W48" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="X48" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y48" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G49" s="16">
+        <v>1</v>
+      </c>
+      <c r="H49" s="16">
+        <v>1</v>
+      </c>
+      <c r="I49" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" s="12">
+        <v>60</v>
+      </c>
+      <c r="K49" s="12">
+        <v>4</v>
+      </c>
+      <c r="L49" s="12">
         <v>5</v>
       </c>
-      <c r="P46" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q46" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="R46" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="S46" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="T46" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U46" s="12">
+      <c r="M49" s="12">
+        <v>69</v>
+      </c>
+      <c r="O49" s="12">
+        <v>1</v>
+      </c>
+      <c r="P49" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q49" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="R49" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="S49" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="T49" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="U49" s="12">
+        <v>25</v>
+      </c>
+      <c r="V49" s="12">
+        <v>126</v>
+      </c>
+      <c r="W49" s="12">
+        <v>69</v>
+      </c>
+      <c r="X49" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="Y49" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G50" s="17">
+        <v>1</v>
+      </c>
+      <c r="H50" s="17">
+        <v>2</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J50" s="18">
+        <v>45</v>
+      </c>
+      <c r="K50" s="18">
+        <v>1</v>
+      </c>
+      <c r="L50" s="18">
+        <v>2</v>
+      </c>
+      <c r="M50" s="12">
+        <v>48</v>
+      </c>
+      <c r="O50" s="12">
+        <v>2</v>
+      </c>
+      <c r="P50" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q50" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="R50" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="S50" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="T50" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="U50" s="12">
+        <v>26</v>
+      </c>
+      <c r="V50" s="12">
+        <v>62</v>
+      </c>
+      <c r="W50" s="12">
+        <v>48</v>
+      </c>
+      <c r="X50" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y50" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G51" s="16">
+        <v>2</v>
+      </c>
+      <c r="H51" s="16">
+        <v>1</v>
+      </c>
+      <c r="I51" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J51" s="12">
         <v>30</v>
       </c>
-      <c r="V46" s="12">
-        <v>2</v>
-      </c>
-      <c r="W46" s="12">
-        <v>1</v>
-      </c>
-      <c r="X46" s="12">
-        <v>1</v>
-      </c>
-      <c r="Y46" s="12">
+      <c r="K51" s="12">
+        <v>1</v>
+      </c>
+      <c r="L51" s="12">
+        <v>3</v>
+      </c>
+      <c r="M51" s="12">
+        <v>34</v>
+      </c>
+      <c r="O51" s="12">
+        <v>3</v>
+      </c>
+      <c r="P51" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q51" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="R51" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="S51" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="T51" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="U51" s="18">
+        <v>26</v>
+      </c>
+      <c r="V51" s="18">
+        <v>62</v>
+      </c>
+      <c r="W51" s="18">
+        <v>34</v>
+      </c>
+      <c r="X51" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y51" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="G52" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="35"/>
+      <c r="M52" s="19">
+        <f>SUM(M49:M51)</f>
+        <v>151</v>
+      </c>
+      <c r="O52" s="12">
+        <v>4</v>
+      </c>
+      <c r="P52" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q52" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="R52" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="S52" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="T52" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="U52" s="18">
+        <v>28</v>
+      </c>
+      <c r="V52" s="18">
+        <v>14</v>
+      </c>
+      <c r="W52" s="18">
+        <v>10</v>
+      </c>
+      <c r="X52" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="7:25" x14ac:dyDescent="0.25">
+      <c r="O53" s="12">
+        <v>5</v>
+      </c>
+      <c r="P53" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q53" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="R53" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="S53" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="T53" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="U53" s="12">
+        <v>30</v>
+      </c>
+      <c r="V53" s="12">
+        <v>2</v>
+      </c>
+      <c r="W53" s="12">
+        <v>1</v>
+      </c>
+      <c r="X53" s="12">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="G47:M47"/>
+    <mergeCell ref="G52:L52"/>
+    <mergeCell ref="G34:L34"/>
+    <mergeCell ref="G36:M36"/>
+    <mergeCell ref="G40:L40"/>
+    <mergeCell ref="G42:M42"/>
+    <mergeCell ref="G45:L45"/>
     <mergeCell ref="G30:M30"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="G2:M2"/>
@@ -6623,12 +6693,8 @@
     <mergeCell ref="G22:L22"/>
     <mergeCell ref="G24:M24"/>
     <mergeCell ref="G28:L28"/>
-    <mergeCell ref="G34:L34"/>
-    <mergeCell ref="G36:M36"/>
-    <mergeCell ref="G40:L40"/>
-    <mergeCell ref="G42:M42"/>
-    <mergeCell ref="G45:L45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>